<commit_message>
ajout de l'initialization automatique des données de la base selon les fichiers du dossier admin, ajcréation des fiches de matières et semestres de tout le dut informatique, ajout de la création des fichiers json de tous les étudiant, de toutes leurs notes ainsi que de leur moyenne dans les ues et les semestres
</commit_message>
<xml_diff>
--- a/projetS5/public/INFO/2018-2019/INFO2/S3/UE31/APA.xlsx
+++ b/projetS5/public/INFO/2018-2019/INFO2/S3/UE31/APA.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdcde\Music\PROJET S5 LPDIOC GESTION ETUDIANT\GestionEtudiants2018\projetS5\public\INFO\2018-2019\INFO2\S3\UE31\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB4CD15-F2FB-4144-B0BC-205E3456840E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="APA" sheetId="1" r:id="rId1"/>
+    <sheet name="APA" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="114">
   <si>
     <t>Numéro</t>
   </si>
@@ -35,6 +30,9 @@
   </si>
   <si>
     <t>Moyenne de l'étudiant</t>
+  </si>
+  <si>
+    <t>Rang</t>
   </si>
   <si>
     <t>BAUDELET</t>
@@ -364,10 +362,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -377,37 +380,28 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -697,23 +691,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E63"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="11.711426" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="25.85083" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -729,1046 +726,1059 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>20150926</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>20150927</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>20150928</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>20150929</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>20150930</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>20150931</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>20150932</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>20150933</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>20150934</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>20150935</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>20150936</v>
       </c>
       <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>20150937</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>20150938</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15">
         <v>7</v>
       </c>
-      <c r="E15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>20150939</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E16">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>20150940</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>20150941</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E18">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>20150942</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>20150943</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>20150944</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E21">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>20150945</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E22">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>20150946</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E23">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>20150947</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E24">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>20150948</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E25">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>20150949</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E26">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>20150950</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>20150951</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E28">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>20150952</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E29">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>20150953</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E30">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>20150954</v>
       </c>
       <c r="B31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E31">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>20150955</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E32">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>20150956</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E33">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>20150957</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E34">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>20150958</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E35">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>20150959</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E36">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>20150960</v>
       </c>
       <c r="B37" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E37">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>20150961</v>
       </c>
       <c r="B38" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E38">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>20150962</v>
       </c>
       <c r="B39" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E39">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>20150963</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E40">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>20150964</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E41">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>20150965</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E42">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>20150966</v>
       </c>
       <c r="B43" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C43" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E43">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>20150967</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E44">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>20150968</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E45">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>20150969</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E46">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>20150970</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E47">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>20150971</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C48" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E48">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>20150972</v>
       </c>
       <c r="B49" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E49">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>20150973</v>
       </c>
       <c r="B50" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E50">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>20150974</v>
       </c>
       <c r="B51" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C51" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D51" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E51">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>20150975</v>
       </c>
       <c r="B52" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E52">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53">
         <v>20150976</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E53">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54">
         <v>20150977</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C54" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D54" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E54">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55">
         <v>20150978</v>
       </c>
       <c r="B55" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D55" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E55">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56">
         <v>20150979</v>
       </c>
       <c r="B56" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E56">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57">
         <v>20150980</v>
       </c>
       <c r="B57" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C57" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E57">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58">
         <v>20150981</v>
       </c>
       <c r="B58" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C58" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E58">
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6">
       <c r="A59">
         <v>20150982</v>
       </c>
       <c r="B59" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C59" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E59">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60">
         <v>20150983</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C60" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E60">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61">
         <v>20150984</v>
       </c>
       <c r="B61" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C61" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61">
         <v>10</v>
       </c>
-      <c r="E61">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62">
         <v>20150985</v>
       </c>
       <c r="B62" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C62" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E62">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63">
         <v>20150986</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C63" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E63">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>